<commit_message>
added excel new property
</commit_message>
<xml_diff>
--- a/src/main/MainResources/ExecutableDriver/UserInput.xlsx
+++ b/src/main/MainResources/ExecutableDriver/UserInput.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepak.kumar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\baseProject\src\main\MainResources\ExecutableDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,6 +23,143 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+  <si>
+    <t>Method43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1  </t>
+  </si>
+  <si>
+    <t>opt 1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>opt 2</t>
+  </si>
+  <si>
+    <t>opt 3</t>
+  </si>
+  <si>
+    <t>res1</t>
+  </si>
+  <si>
+    <t>res2</t>
+  </si>
+  <si>
+    <t>res3</t>
+  </si>
+  <si>
+    <t>Method44</t>
+  </si>
+  <si>
+    <t>Method45</t>
+  </si>
+  <si>
+    <t>test21</t>
+  </si>
+  <si>
+    <t>test22</t>
+  </si>
+  <si>
+    <t>test23</t>
+  </si>
+  <si>
+    <t>test24</t>
+  </si>
+  <si>
+    <t>test25</t>
+  </si>
+  <si>
+    <t>opt 21</t>
+  </si>
+  <si>
+    <t>opt 22</t>
+  </si>
+  <si>
+    <t>opt 23</t>
+  </si>
+  <si>
+    <t>opt 24</t>
+  </si>
+  <si>
+    <t>opt 25</t>
+  </si>
+  <si>
+    <t>res21</t>
+  </si>
+  <si>
+    <t>res22</t>
+  </si>
+  <si>
+    <t>res23</t>
+  </si>
+  <si>
+    <t>res24</t>
+  </si>
+  <si>
+    <t>res25</t>
+  </si>
+  <si>
+    <t>pass1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">case1 </t>
+  </si>
+  <si>
+    <t>query1</t>
+  </si>
+  <si>
+    <t>pass2</t>
+  </si>
+  <si>
+    <t>pass3</t>
+  </si>
+  <si>
+    <t>pass4</t>
+  </si>
+  <si>
+    <t>pass5</t>
+  </si>
+  <si>
+    <t>case2</t>
+  </si>
+  <si>
+    <t>case3</t>
+  </si>
+  <si>
+    <t>case4</t>
+  </si>
+  <si>
+    <t>case5</t>
+  </si>
+  <si>
+    <t>query2</t>
+  </si>
+  <si>
+    <t>query3</t>
+  </si>
+  <si>
+    <t>query4</t>
+  </si>
+  <si>
+    <t>query5</t>
+  </si>
+  <si>
+    <t>Method46</t>
+  </si>
+  <si>
+    <t>Method47</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
@@ -34,12 +171,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -54,8 +196,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +483,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="A5:C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>